<commit_message>
Implemented the mask size changes in the calibration condition file.
</commit_message>
<xml_diff>
--- a/subjs-mc3.xlsx
+++ b/subjs-mc3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="23060" yWindow="10680" windowWidth="15200" windowHeight="10000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mc" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
   <si>
     <t>l</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>divergent staircases; excluded</t>
+  </si>
+  <si>
+    <t>Azman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Zhi Wei</t>
   </si>
 </sst>
 </file>
@@ -285,7 +294,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -457,6 +466,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -515,7 +526,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="185">
     <cellStyle name="Bad" xfId="151" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Comma" xfId="145" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -607,6 +618,7 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="150" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -697,6 +709,7 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="170" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2337,7 +2350,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2449,13 +2462,41 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-0.79700000000000004</v>
+      </c>
+      <c r="D3">
+        <v>-0.35199999999999998</v>
+      </c>
+      <c r="E3">
+        <v>-0.877</v>
+      </c>
+      <c r="F3">
+        <v>-0.19800000000000001</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3" si="2">AVERAGE(C3,D3)</f>
+        <v>-0.57450000000000001</v>
+      </c>
+      <c r="H3" s="6">
+        <f t="shared" ref="H3" si="3">AVERAGE(E3,F3)</f>
+        <v>-0.53749999999999998</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
@@ -2466,13 +2507,38 @@
       <c r="S3"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>-1.0569999999999999</v>
+      </c>
+      <c r="D4">
+        <v>-0.95799999999999996</v>
+      </c>
+      <c r="E4">
+        <v>-0.997</v>
+      </c>
+      <c r="F4">
+        <v>-1.212</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" ref="G4" si="4">AVERAGE(C4,D4)</f>
+        <v>-1.0074999999999998</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4" si="5">AVERAGE(E4,F4)</f>
+        <v>-1.1045</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>

</xml_diff>

<commit_message>
New data. Switched to no-fixation paradigm to further approximate the BR scenario.
</commit_message>
<xml_diff>
--- a/subjs-mc3.xlsx
+++ b/subjs-mc3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="51">
   <si>
     <t>l</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>Zhi Wei</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>Jois Cham</t>
+  </si>
+  <si>
+    <t>Frances</t>
   </si>
 </sst>
 </file>
@@ -2350,7 +2359,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2549,13 +2558,38 @@
       <c r="S4"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>-1.022</v>
+      </c>
+      <c r="D5">
+        <v>-0.95799999999999996</v>
+      </c>
+      <c r="E5">
+        <v>-1.1120000000000001</v>
+      </c>
+      <c r="F5">
+        <v>-1.0780000000000001</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" ref="G5" si="6">AVERAGE(C5,D5)</f>
+        <v>-0.99</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" ref="H5" si="7">AVERAGE(E5,F5)</f>
+        <v>-1.0950000000000002</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>48</v>
+      </c>
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5"/>
@@ -2566,13 +2600,38 @@
       <c r="S5"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>-0.91700000000000004</v>
+      </c>
+      <c r="D6">
+        <v>-0.89200000000000002</v>
+      </c>
+      <c r="E6">
+        <v>-0.84199999999999997</v>
+      </c>
+      <c r="F6">
+        <v>-0.85799999999999998</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" ref="G6" si="8">AVERAGE(C6,D6)</f>
+        <v>-0.90450000000000008</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" ref="H6" si="9">AVERAGE(E6,F6)</f>
+        <v>-0.85</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>49</v>
+      </c>
       <c r="L6"/>
       <c r="M6"/>
       <c r="N6"/>
@@ -2583,13 +2642,38 @@
       <c r="S6"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>-0.96199999999999997</v>
+      </c>
+      <c r="D7">
+        <v>-0.95199999999999996</v>
+      </c>
+      <c r="E7">
+        <v>-1.1419999999999999</v>
+      </c>
+      <c r="F7">
+        <v>-1.212</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" ref="G7" si="10">AVERAGE(C7,D7)</f>
+        <v>-0.95699999999999996</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" ref="H7" si="11">AVERAGE(E7,F7)</f>
+        <v>-1.177</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>50</v>
+      </c>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>

</xml_diff>